<commit_message>
Datos organizados en un solo array
</commit_message>
<xml_diff>
--- a/Date/Medicion 11-03.xlsx
+++ b/Date/Medicion 11-03.xlsx
@@ -1,37 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\4. Resultados\4.1 Mediciones\Mediciones acumulador completo\11-03-2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Administrador\Angel\LIBROS\Machine Learning\st-acumulador\Date\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E440E52-78E0-4CB7-BD2E-686F075DFDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0BB3C4-8941-412A-84B6-36BD37FFE63D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TMB010rfrf01" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="19">
   <si>
     <t>Place</t>
   </si>
@@ -82,9 +71,6 @@
   </si>
   <si>
     <t>CARGA CLOSE CIRCUIT</t>
-  </si>
-  <si>
-    <t>FAN ON</t>
   </si>
   <si>
     <t>Tout</t>
@@ -580,7 +566,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -588,6 +574,7 @@
     <xf numFmtId="14" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="21" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -711,7 +698,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4735,7 +4722,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="32416816"/>
@@ -4796,7 +4783,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="369655288"/>
@@ -4839,7 +4826,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4869,7 +4856,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4945,7 +4932,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -8971,7 +8958,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="369377872"/>
@@ -9032,7 +9019,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="368471712"/>
@@ -9075,7 +9062,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -9105,7 +9092,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9186,7 +9173,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -14552,7 +14539,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="369347792"/>
@@ -14613,7 +14600,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="369189216"/>
@@ -14656,7 +14643,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -14686,7 +14673,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -14762,7 +14749,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -18784,7 +18771,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="369986784"/>
@@ -18845,7 +18832,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="369989136"/>
@@ -18888,7 +18875,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -18918,7 +18905,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -21573,16 +21560,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S531"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B487" workbookViewId="0">
-      <selection activeCell="C505" sqref="C505"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -21629,13 +21616,13 @@
         <v>13</v>
       </c>
       <c r="P1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -21662,7 +21649,7 @@
         <v>34.761800000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -21716,7 +21703,7 @@
         <v>34.994399999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -21770,7 +21757,7 @@
         <v>35.2258</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -21824,7 +21811,7 @@
         <v>35.455999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -21878,7 +21865,7 @@
         <v>35.685000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -21932,7 +21919,7 @@
         <v>35.912799999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -21986,11 +21973,11 @@
         <v>36.139400000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="7">
         <v>36528</v>
       </c>
       <c r="C9" s="2">
@@ -22040,7 +22027,7 @@
         <v>36.364800000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -22094,12 +22081,12 @@
         <v>36.588999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>17</v>
+      <c r="B11" s="1">
+        <v>36528</v>
       </c>
       <c r="C11" s="5">
         <v>0.40138888888888902</v>
@@ -22148,7 +22135,7 @@
         <v>36.811999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -22202,7 +22189,7 @@
         <v>37.033799999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -22256,7 +22243,7 @@
         <v>37.254399999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -22313,7 +22300,7 @@
         <v>37.473799999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -22370,7 +22357,7 @@
         <v>37.692</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -22427,7 +22414,7 @@
         <v>37.908999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -22484,7 +22471,7 @@
         <v>38.1248</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -22541,7 +22528,7 @@
         <v>38.339399999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -22598,7 +22585,7 @@
         <v>38.552799999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -22655,7 +22642,7 @@
         <v>38.765000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -22712,7 +22699,7 @@
         <v>38.975999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -22769,7 +22756,7 @@
         <v>39.1858</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -22826,7 +22813,7 @@
         <v>39.394399999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -22883,7 +22870,7 @@
         <v>39.601799999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -22940,7 +22927,7 @@
         <v>39.808</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -22997,7 +22984,7 @@
         <v>40.012999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -23054,7 +23041,7 @@
         <v>40.216799999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -23111,7 +23098,7 @@
         <v>40.419399999999996</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -23168,7 +23155,7 @@
         <v>40.620800000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -23225,7 +23212,7 @@
         <v>40.820999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -23282,7 +23269,7 @@
         <v>41.019999999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -23339,7 +23326,7 @@
         <v>41.217799999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -23396,7 +23383,7 @@
         <v>41.414400000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -23453,7 +23440,7 @@
         <v>41.6098</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -23510,7 +23497,7 @@
         <v>41.804000000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -23567,7 +23554,7 @@
         <v>41.997</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -23624,7 +23611,7 @@
         <v>42.188800000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -23681,7 +23668,7 @@
         <v>42.379399999999997</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -23738,7 +23725,7 @@
         <v>42.568799999999996</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -23795,7 +23782,7 @@
         <v>42.756999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -23852,7 +23839,7 @@
         <v>42.944000000000003</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -23909,7 +23896,7 @@
         <v>43.129800000000003</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -23966,7 +23953,7 @@
         <v>43.314399999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>16</v>
       </c>
@@ -24023,7 +24010,7 @@
         <v>43.497799999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>16</v>
       </c>
@@ -24080,7 +24067,7 @@
         <v>43.68</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -24137,7 +24124,7 @@
         <v>43.860999999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>16</v>
       </c>
@@ -24194,7 +24181,7 @@
         <v>44.040799999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -24251,7 +24238,7 @@
         <v>44.2194</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -24308,7 +24295,7 @@
         <v>44.396799999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>16</v>
       </c>
@@ -24365,7 +24352,7 @@
         <v>44.573</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>16</v>
       </c>
@@ -24422,7 +24409,7 @@
         <v>44.748000000000005</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -24479,7 +24466,7 @@
         <v>44.921800000000005</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>16</v>
       </c>
@@ -24536,7 +24523,7 @@
         <v>45.0944</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -24593,7 +24580,7 @@
         <v>45.265799999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>16</v>
       </c>
@@ -24650,7 +24637,7 @@
         <v>45.436</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>16</v>
       </c>
@@ -24707,7 +24694,7 @@
         <v>45.604999999999997</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>16</v>
       </c>
@@ -24764,7 +24751,7 @@
         <v>45.772800000000004</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>16</v>
       </c>
@@ -24821,7 +24808,7 @@
         <v>45.939399999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>16</v>
       </c>
@@ -24878,7 +24865,7 @@
         <v>46.104799999999997</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>16</v>
       </c>
@@ -24935,7 +24922,7 @@
         <v>46.268999999999998</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -24992,7 +24979,7 @@
         <v>46.432000000000002</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>16</v>
       </c>
@@ -25049,7 +25036,7 @@
         <v>46.593800000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>16</v>
       </c>
@@ -25106,7 +25093,7 @@
         <v>46.754400000000004</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>16</v>
       </c>
@@ -25163,7 +25150,7 @@
         <v>46.913800000000002</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>16</v>
       </c>
@@ -25220,7 +25207,7 @@
         <v>47.072000000000003</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>16</v>
       </c>
@@ -25277,7 +25264,7 @@
         <v>47.228999999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>16</v>
       </c>
@@ -25334,7 +25321,7 @@
         <v>47.384799999999998</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>16</v>
       </c>
@@ -25391,7 +25378,7 @@
         <v>47.539400000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>16</v>
       </c>
@@ -25448,7 +25435,7 @@
         <v>47.692799999999998</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>16</v>
       </c>
@@ -25505,7 +25492,7 @@
         <v>47.844999999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>16</v>
       </c>
@@ -25562,7 +25549,7 @@
         <v>47.995999999999995</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>16</v>
       </c>
@@ -25619,7 +25606,7 @@
         <v>48.145800000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>16</v>
       </c>
@@ -25676,7 +25663,7 @@
         <v>48.294399999999996</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>16</v>
       </c>
@@ -25733,7 +25720,7 @@
         <v>48.441800000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>16</v>
       </c>
@@ -25790,7 +25777,7 @@
         <v>48.588000000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>16</v>
       </c>
@@ -25847,7 +25834,7 @@
         <v>48.732999999999997</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>16</v>
       </c>
@@ -25904,7 +25891,7 @@
         <v>48.876800000000003</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>16</v>
       </c>
@@ -25961,7 +25948,7 @@
         <v>49.019399999999997</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>16</v>
       </c>
@@ -26018,7 +26005,7 @@
         <v>49.160800000000002</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>16</v>
       </c>
@@ -26075,7 +26062,7 @@
         <v>49.301000000000002</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>16</v>
       </c>
@@ -26132,7 +26119,7 @@
         <v>49.44</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>16</v>
       </c>
@@ -26189,7 +26176,7 @@
         <v>49.577799999999996</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>16</v>
       </c>
@@ -26246,7 +26233,7 @@
         <v>49.714399999999998</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>16</v>
       </c>
@@ -26303,7 +26290,7 @@
         <v>49.849800000000002</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>16</v>
       </c>
@@ -26360,7 +26347,7 @@
         <v>49.983999999999995</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>16</v>
       </c>
@@ -26417,7 +26404,7 @@
         <v>50.117000000000004</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>16</v>
       </c>
@@ -26474,7 +26461,7 @@
         <v>50.248800000000003</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>16</v>
       </c>
@@ -26531,7 +26518,7 @@
         <v>50.379400000000004</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>16</v>
       </c>
@@ -26588,7 +26575,7 @@
         <v>50.508800000000001</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>16</v>
       </c>
@@ -26645,7 +26632,7 @@
         <v>50.637</v>
       </c>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>16</v>
       </c>
@@ -26702,7 +26689,7 @@
         <v>50.763999999999996</v>
       </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>16</v>
       </c>
@@ -26759,7 +26746,7 @@
         <v>50.889800000000001</v>
       </c>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>16</v>
       </c>
@@ -26816,7 +26803,7 @@
         <v>51.014400000000002</v>
       </c>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>16</v>
       </c>
@@ -26873,7 +26860,7 @@
         <v>51.137799999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>16</v>
       </c>
@@ -26930,7 +26917,7 @@
         <v>51.260000000000005</v>
       </c>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>16</v>
       </c>
@@ -26987,7 +26974,7 @@
         <v>51.381</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>16</v>
       </c>
@@ -27044,7 +27031,7 @@
         <v>51.500799999999998</v>
       </c>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>16</v>
       </c>
@@ -27101,7 +27088,7 @@
         <v>51.619399999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>16</v>
       </c>
@@ -27158,7 +27145,7 @@
         <v>51.736800000000002</v>
       </c>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>16</v>
       </c>
@@ -27215,7 +27202,7 @@
         <v>51.852999999999994</v>
       </c>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>16</v>
       </c>
@@ -27272,7 +27259,7 @@
         <v>51.968000000000004</v>
       </c>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>16</v>
       </c>
@@ -27329,7 +27316,7 @@
         <v>52.081800000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>16</v>
       </c>
@@ -27386,7 +27373,7 @@
         <v>52.194400000000002</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>16</v>
       </c>
@@ -27443,7 +27430,7 @@
         <v>52.305800000000005</v>
       </c>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>16</v>
       </c>
@@ -27500,7 +27487,7 @@
         <v>52.415999999999997</v>
       </c>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>16</v>
       </c>
@@ -27557,7 +27544,7 @@
         <v>52.525000000000006</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>16</v>
       </c>
@@ -27614,7 +27601,7 @@
         <v>52.632800000000003</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>16</v>
       </c>
@@ -27671,7 +27658,7 @@
         <v>52.156199999999998</v>
       </c>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>16</v>
       </c>
@@ -27728,7 +27715,7 @@
         <v>52.250749999999996</v>
       </c>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>16</v>
       </c>
@@ -27785,7 +27772,7 @@
         <v>52.344000000000001</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>16</v>
       </c>
@@ -27842,7 +27829,7 @@
         <v>52.435950000000005</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>16</v>
       </c>
@@ -27899,7 +27886,7 @@
         <v>52.526600000000002</v>
       </c>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>16</v>
       </c>
@@ -27956,7 +27943,7 @@
         <v>52.615949999999998</v>
       </c>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>16</v>
       </c>
@@ -28013,7 +28000,7 @@
         <v>52.704000000000001</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>16</v>
       </c>
@@ -28070,7 +28057,7 @@
         <v>52.790750000000003</v>
       </c>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>16</v>
       </c>
@@ -28127,7 +28114,7 @@
         <v>52.876199999999997</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>16</v>
       </c>
@@ -28184,7 +28171,7 @@
         <v>52.960350000000005</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>16</v>
       </c>
@@ -28241,7 +28228,7 @@
         <v>53.043199999999999</v>
       </c>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>16</v>
       </c>
@@ -28298,7 +28285,7 @@
         <v>53.124749999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>16</v>
       </c>
@@ -28355,7 +28342,7 @@
         <v>53.204999999999998</v>
       </c>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>16</v>
       </c>
@@ -28412,7 +28399,7 @@
         <v>53.283949999999997</v>
       </c>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>16</v>
       </c>
@@ -28469,7 +28456,7 @@
         <v>53.361600000000003</v>
       </c>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>16</v>
       </c>
@@ -28526,7 +28513,7 @@
         <v>53.437950000000001</v>
       </c>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>16</v>
       </c>
@@ -28583,7 +28570,7 @@
         <v>53.513000000000005</v>
       </c>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>16</v>
       </c>
@@ -28640,7 +28627,7 @@
         <v>53.586749999999995</v>
       </c>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>16</v>
       </c>
@@ -28697,7 +28684,7 @@
         <v>53.659199999999998</v>
       </c>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>16</v>
       </c>
@@ -28754,7 +28741,7 @@
         <v>53.730350000000001</v>
       </c>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>16</v>
       </c>
@@ -28811,7 +28798,7 @@
         <v>53.800200000000004</v>
       </c>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>16</v>
       </c>
@@ -28868,7 +28855,7 @@
         <v>53.868750000000006</v>
       </c>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>16</v>
       </c>
@@ -28925,7 +28912,7 @@
         <v>53.936</v>
       </c>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>16</v>
       </c>
@@ -28982,7 +28969,7 @@
         <v>54.001950000000001</v>
       </c>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>16</v>
       </c>
@@ -29039,7 +29026,7 @@
         <v>54.066600000000001</v>
       </c>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>16</v>
       </c>
@@ -29096,7 +29083,7 @@
         <v>54.129950000000001</v>
       </c>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>16</v>
       </c>
@@ -29153,7 +29140,7 @@
         <v>54.192</v>
       </c>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>16</v>
       </c>
@@ -29210,7 +29197,7 @@
         <v>54.252749999999999</v>
       </c>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>16</v>
       </c>
@@ -29267,7 +29254,7 @@
         <v>54.312200000000004</v>
       </c>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>16</v>
       </c>
@@ -29324,7 +29311,7 @@
         <v>54.370350000000002</v>
       </c>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>16</v>
       </c>
@@ -29381,7 +29368,7 @@
         <v>54.427199999999999</v>
       </c>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>16</v>
       </c>
@@ -29438,7 +29425,7 @@
         <v>54.482750000000003</v>
       </c>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>16</v>
       </c>
@@ -29495,7 +29482,7 @@
         <v>54.536999999999999</v>
       </c>
     </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>16</v>
       </c>
@@ -29552,7 +29539,7 @@
         <v>54.589950000000002</v>
       </c>
     </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>16</v>
       </c>
@@ -29609,7 +29596,7 @@
         <v>54.641599999999997</v>
       </c>
     </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>16</v>
       </c>
@@ -29666,7 +29653,7 @@
         <v>54.691950000000006</v>
       </c>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>16</v>
       </c>
@@ -29723,7 +29710,7 @@
         <v>54.741</v>
       </c>
     </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>16</v>
       </c>
@@ -29780,7 +29767,7 @@
         <v>54.78875</v>
       </c>
     </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>16</v>
       </c>
@@ -29837,7 +29824,7 @@
         <v>54.8352</v>
       </c>
     </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>16</v>
       </c>
@@ -29894,7 +29881,7 @@
         <v>54.88035</v>
       </c>
     </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>16</v>
       </c>
@@ -29951,7 +29938,7 @@
         <v>54.924199999999999</v>
       </c>
     </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>16</v>
       </c>
@@ -30008,7 +29995,7 @@
         <v>54.966749999999998</v>
       </c>
     </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>16</v>
       </c>
@@ -30065,7 +30052,7 @@
         <v>55.008000000000003</v>
       </c>
     </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>16</v>
       </c>
@@ -30122,7 +30109,7 @@
         <v>55.04795</v>
       </c>
     </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>16</v>
       </c>
@@ -30179,7 +30166,7 @@
         <v>55.086599999999997</v>
       </c>
     </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>16</v>
       </c>
@@ -30236,7 +30223,7 @@
         <v>55.123949999999994</v>
       </c>
     </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>16</v>
       </c>
@@ -30293,7 +30280,7 @@
         <v>55.160000000000004</v>
       </c>
     </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>16</v>
       </c>
@@ -30350,7 +30337,7 @@
         <v>55.194749999999999</v>
       </c>
     </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>16</v>
       </c>
@@ -30407,7 +30394,7 @@
         <v>55.228200000000001</v>
       </c>
     </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>16</v>
       </c>
@@ -30464,7 +30451,7 @@
         <v>55.260350000000003</v>
       </c>
     </row>
-    <row r="158" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>16</v>
       </c>
@@ -30521,7 +30508,7 @@
         <v>55.291200000000003</v>
       </c>
     </row>
-    <row r="159" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>16</v>
       </c>
@@ -30578,7 +30565,7 @@
         <v>55.320750000000004</v>
       </c>
     </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>16</v>
       </c>
@@ -30635,7 +30622,7 @@
         <v>55.348999999999997</v>
       </c>
     </row>
-    <row r="161" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>16</v>
       </c>
@@ -30692,7 +30679,7 @@
         <v>55.375950000000003</v>
       </c>
     </row>
-    <row r="162" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>16</v>
       </c>
@@ -30749,7 +30736,7 @@
         <v>55.401600000000002</v>
       </c>
     </row>
-    <row r="163" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>16</v>
       </c>
@@ -30806,7 +30793,7 @@
         <v>55.42595</v>
       </c>
     </row>
-    <row r="164" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>16</v>
       </c>
@@ -30863,7 +30850,7 @@
         <v>55.448999999999998</v>
       </c>
     </row>
-    <row r="165" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>16</v>
       </c>
@@ -30920,7 +30907,7 @@
         <v>55.470750000000002</v>
       </c>
     </row>
-    <row r="166" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>16</v>
       </c>
@@ -30977,7 +30964,7 @@
         <v>55.491199999999999</v>
       </c>
     </row>
-    <row r="167" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>16</v>
       </c>
@@ -31034,7 +31021,7 @@
         <v>55.510350000000003</v>
       </c>
     </row>
-    <row r="168" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>16</v>
       </c>
@@ -31091,7 +31078,7 @@
         <v>55.528200000000005</v>
       </c>
     </row>
-    <row r="169" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>16</v>
       </c>
@@ -31148,7 +31135,7 @@
         <v>55.544750000000008</v>
       </c>
     </row>
-    <row r="170" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>16</v>
       </c>
@@ -31205,7 +31192,7 @@
         <v>55.56</v>
       </c>
     </row>
-    <row r="171" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>16</v>
       </c>
@@ -31262,7 +31249,7 @@
         <v>55.573949999999996</v>
       </c>
     </row>
-    <row r="172" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>16</v>
       </c>
@@ -31319,7 +31306,7 @@
         <v>55.586600000000004</v>
       </c>
     </row>
-    <row r="173" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>16</v>
       </c>
@@ -31376,7 +31363,7 @@
         <v>55.597949999999997</v>
       </c>
     </row>
-    <row r="174" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>16</v>
       </c>
@@ -31433,7 +31420,7 @@
         <v>55.608000000000004</v>
       </c>
     </row>
-    <row r="175" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>16</v>
       </c>
@@ -31490,7 +31477,7 @@
         <v>55.616750000000003</v>
       </c>
     </row>
-    <row r="176" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>16</v>
       </c>
@@ -31547,7 +31534,7 @@
         <v>55.624200000000002</v>
       </c>
     </row>
-    <row r="177" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>16</v>
       </c>
@@ -31604,7 +31591,7 @@
         <v>55.63035</v>
       </c>
     </row>
-    <row r="178" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>16</v>
       </c>
@@ -31661,7 +31648,7 @@
         <v>55.635199999999998</v>
       </c>
     </row>
-    <row r="179" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>16</v>
       </c>
@@ -31718,7 +31705,7 @@
         <v>55.638750000000002</v>
       </c>
     </row>
-    <row r="180" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>16</v>
       </c>
@@ -31775,7 +31762,7 @@
         <v>55.641000000000005</v>
       </c>
     </row>
-    <row r="181" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>16</v>
       </c>
@@ -31832,7 +31819,7 @@
         <v>55.641950000000001</v>
       </c>
     </row>
-    <row r="182" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>16</v>
       </c>
@@ -31889,7 +31876,7 @@
         <v>55.641599999999997</v>
       </c>
     </row>
-    <row r="183" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>16</v>
       </c>
@@ -31946,7 +31933,7 @@
         <v>55.639949999999999</v>
       </c>
     </row>
-    <row r="184" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>16</v>
       </c>
@@ -32003,7 +31990,7 @@
         <v>55.637</v>
       </c>
     </row>
-    <row r="185" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>16</v>
       </c>
@@ -32060,7 +32047,7 @@
         <v>55.632750000000001</v>
       </c>
     </row>
-    <row r="186" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>16</v>
       </c>
@@ -32117,7 +32104,7 @@
         <v>55.627200000000002</v>
       </c>
     </row>
-    <row r="187" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>16</v>
       </c>
@@ -32174,7 +32161,7 @@
         <v>55.620350000000002</v>
       </c>
     </row>
-    <row r="188" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>16</v>
       </c>
@@ -32231,7 +32218,7 @@
         <v>55.612200000000001</v>
       </c>
     </row>
-    <row r="189" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>16</v>
       </c>
@@ -32288,7 +32275,7 @@
         <v>55.60275</v>
       </c>
     </row>
-    <row r="190" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>16</v>
       </c>
@@ -32338,7 +32325,7 @@
         <v>73.5</v>
       </c>
     </row>
-    <row r="191" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>16</v>
       </c>
@@ -32388,7 +32375,7 @@
         <v>73.7</v>
       </c>
     </row>
-    <row r="192" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>16</v>
       </c>
@@ -32438,7 +32425,7 @@
         <v>73.7</v>
       </c>
     </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>16</v>
       </c>
@@ -32488,7 +32475,7 @@
         <v>73.7</v>
       </c>
     </row>
-    <row r="194" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>16</v>
       </c>
@@ -32538,7 +32525,7 @@
         <v>73.900000000000006</v>
       </c>
     </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>16</v>
       </c>
@@ -32588,7 +32575,7 @@
         <v>73.599999999999994</v>
       </c>
     </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>16</v>
       </c>
@@ -32638,7 +32625,7 @@
         <v>73.5</v>
       </c>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>16</v>
       </c>
@@ -32688,7 +32675,7 @@
         <v>73.599999999999994</v>
       </c>
     </row>
-    <row r="198" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>16</v>
       </c>
@@ -32738,7 +32725,7 @@
         <v>73.8</v>
       </c>
     </row>
-    <row r="199" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>16</v>
       </c>
@@ -32788,7 +32775,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="200" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>16</v>
       </c>
@@ -32838,7 +32825,7 @@
         <v>74.400000000000006</v>
       </c>
     </row>
-    <row r="201" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>16</v>
       </c>
@@ -32888,7 +32875,7 @@
         <v>75.099999999999994</v>
       </c>
     </row>
-    <row r="202" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>16</v>
       </c>
@@ -32938,7 +32925,7 @@
         <v>74.8</v>
       </c>
     </row>
-    <row r="203" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>16</v>
       </c>
@@ -32988,7 +32975,7 @@
         <v>73.900000000000006</v>
       </c>
     </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>16</v>
       </c>
@@ -33038,7 +33025,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="205" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>16</v>
       </c>
@@ -33088,7 +33075,7 @@
         <v>73.900000000000006</v>
       </c>
     </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>16</v>
       </c>
@@ -33138,7 +33125,7 @@
         <v>74.3</v>
       </c>
     </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>16</v>
       </c>
@@ -33188,7 +33175,7 @@
         <v>74.2</v>
       </c>
     </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>16</v>
       </c>
@@ -33238,7 +33225,7 @@
         <v>74.599999999999994</v>
       </c>
     </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>16</v>
       </c>
@@ -33288,7 +33275,7 @@
         <v>74.900000000000006</v>
       </c>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>16</v>
       </c>
@@ -33338,7 +33325,7 @@
         <v>74.5</v>
       </c>
     </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>16</v>
       </c>
@@ -33388,7 +33375,7 @@
         <v>74.599999999999994</v>
       </c>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>16</v>
       </c>
@@ -33438,7 +33425,7 @@
         <v>70.900000000000006</v>
       </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>16</v>
       </c>
@@ -33488,7 +33475,7 @@
         <v>67.400000000000006</v>
       </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>16</v>
       </c>
@@ -33538,7 +33525,7 @@
         <v>66.7</v>
       </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>16</v>
       </c>
@@ -33588,7 +33575,7 @@
         <v>68.8</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>16</v>
       </c>
@@ -33638,7 +33625,7 @@
         <v>69.900000000000006</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>16</v>
       </c>
@@ -33688,7 +33675,7 @@
         <v>70.8</v>
       </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>16</v>
       </c>
@@ -33738,7 +33725,7 @@
         <v>71.599999999999994</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>16</v>
       </c>
@@ -33788,7 +33775,7 @@
         <v>72.3</v>
       </c>
     </row>
-    <row r="220" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>16</v>
       </c>
@@ -33838,7 +33825,7 @@
         <v>72.7</v>
       </c>
     </row>
-    <row r="221" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>16</v>
       </c>
@@ -33888,7 +33875,7 @@
         <v>72.7</v>
       </c>
     </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>16</v>
       </c>
@@ -33938,7 +33925,7 @@
         <v>72.8</v>
       </c>
     </row>
-    <row r="223" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>16</v>
       </c>
@@ -33988,7 +33975,7 @@
         <v>72.2</v>
       </c>
     </row>
-    <row r="224" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>16</v>
       </c>
@@ -34038,7 +34025,7 @@
         <v>72.2</v>
       </c>
     </row>
-    <row r="225" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>16</v>
       </c>
@@ -34088,7 +34075,7 @@
         <v>72.7</v>
       </c>
     </row>
-    <row r="226" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>16</v>
       </c>
@@ -34138,7 +34125,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="227" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>16</v>
       </c>
@@ -34188,7 +34175,7 @@
         <v>73.599999999999994</v>
       </c>
     </row>
-    <row r="228" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>16</v>
       </c>
@@ -34238,7 +34225,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="229" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>16</v>
       </c>
@@ -34288,7 +34275,7 @@
         <v>74.5</v>
       </c>
     </row>
-    <row r="230" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>16</v>
       </c>
@@ -34338,7 +34325,7 @@
         <v>75.099999999999994</v>
       </c>
     </row>
-    <row r="231" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>16</v>
       </c>
@@ -34388,7 +34375,7 @@
         <v>74.599999999999994</v>
       </c>
     </row>
-    <row r="232" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>16</v>
       </c>
@@ -34438,7 +34425,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="233" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>16</v>
       </c>
@@ -34488,7 +34475,7 @@
         <v>75.400000000000006</v>
       </c>
     </row>
-    <row r="234" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>16</v>
       </c>
@@ -34538,7 +34525,7 @@
         <v>75.3</v>
       </c>
     </row>
-    <row r="235" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>16</v>
       </c>
@@ -34588,7 +34575,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="236" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>16</v>
       </c>
@@ -34638,7 +34625,7 @@
         <v>75.7</v>
       </c>
     </row>
-    <row r="237" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>16</v>
       </c>
@@ -34688,7 +34675,7 @@
         <v>75.8</v>
       </c>
     </row>
-    <row r="238" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>16</v>
       </c>
@@ -34738,7 +34725,7 @@
         <v>76.400000000000006</v>
       </c>
     </row>
-    <row r="239" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>16</v>
       </c>
@@ -34788,7 +34775,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="240" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>16</v>
       </c>
@@ -34838,7 +34825,7 @@
         <v>75.7</v>
       </c>
     </row>
-    <row r="241" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>16</v>
       </c>
@@ -34888,7 +34875,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="242" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>16</v>
       </c>
@@ -34938,7 +34925,7 @@
         <v>76.099999999999994</v>
       </c>
     </row>
-    <row r="243" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>16</v>
       </c>
@@ -34988,7 +34975,7 @@
         <v>75.2</v>
       </c>
     </row>
-    <row r="244" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>16</v>
       </c>
@@ -35038,7 +35025,7 @@
         <v>76.099999999999994</v>
       </c>
     </row>
-    <row r="245" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>16</v>
       </c>
@@ -35088,7 +35075,7 @@
         <v>76.2</v>
       </c>
     </row>
-    <row r="246" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>16</v>
       </c>
@@ -35138,7 +35125,7 @@
         <v>76.7</v>
       </c>
     </row>
-    <row r="247" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>16</v>
       </c>
@@ -35188,7 +35175,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="248" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>16</v>
       </c>
@@ -35238,7 +35225,7 @@
         <v>77.599999999999994</v>
       </c>
     </row>
-    <row r="249" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>16</v>
       </c>
@@ -35288,7 +35275,7 @@
         <v>76.900000000000006</v>
       </c>
     </row>
-    <row r="250" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>16</v>
       </c>
@@ -35338,7 +35325,7 @@
         <v>76.7</v>
       </c>
     </row>
-    <row r="251" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>16</v>
       </c>
@@ -35388,7 +35375,7 @@
         <v>76.599999999999994</v>
       </c>
     </row>
-    <row r="252" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>16</v>
       </c>
@@ -35438,7 +35425,7 @@
         <v>76.099999999999994</v>
       </c>
     </row>
-    <row r="253" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>16</v>
       </c>
@@ -35488,7 +35475,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="254" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>16</v>
       </c>
@@ -35538,7 +35525,7 @@
         <v>76.400000000000006</v>
       </c>
     </row>
-    <row r="255" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>16</v>
       </c>
@@ -35588,7 +35575,7 @@
         <v>75.7</v>
       </c>
     </row>
-    <row r="256" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>16</v>
       </c>
@@ -35638,7 +35625,7 @@
         <v>76.3</v>
       </c>
     </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>16</v>
       </c>
@@ -35688,7 +35675,7 @@
         <v>76.599999999999994</v>
       </c>
     </row>
-    <row r="258" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>16</v>
       </c>
@@ -35738,7 +35725,7 @@
         <v>76.599999999999994</v>
       </c>
     </row>
-    <row r="259" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>16</v>
       </c>
@@ -35788,7 +35775,7 @@
         <v>76.5</v>
       </c>
     </row>
-    <row r="260" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>16</v>
       </c>
@@ -35838,7 +35825,7 @@
         <v>76.3</v>
       </c>
     </row>
-    <row r="261" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>16</v>
       </c>
@@ -35888,7 +35875,7 @@
         <v>75.8</v>
       </c>
     </row>
-    <row r="262" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>16</v>
       </c>
@@ -35938,7 +35925,7 @@
         <v>75.900000000000006</v>
       </c>
     </row>
-    <row r="263" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>16</v>
       </c>
@@ -35988,7 +35975,7 @@
         <v>76.099999999999994</v>
       </c>
     </row>
-    <row r="264" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>16</v>
       </c>
@@ -36038,7 +36025,7 @@
         <v>76.5</v>
       </c>
     </row>
-    <row r="265" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>16</v>
       </c>
@@ -36088,7 +36075,7 @@
         <v>77.2</v>
       </c>
     </row>
-    <row r="266" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>16</v>
       </c>
@@ -36138,7 +36125,7 @@
         <v>76.5</v>
       </c>
     </row>
-    <row r="267" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>16</v>
       </c>
@@ -36188,7 +36175,7 @@
         <v>76.400000000000006</v>
       </c>
     </row>
-    <row r="268" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>16</v>
       </c>
@@ -36238,7 +36225,7 @@
         <v>76.2</v>
       </c>
     </row>
-    <row r="269" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>16</v>
       </c>
@@ -36288,7 +36275,7 @@
         <v>76.099999999999994</v>
       </c>
     </row>
-    <row r="270" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>16</v>
       </c>
@@ -36338,7 +36325,7 @@
         <v>75.900000000000006</v>
       </c>
     </row>
-    <row r="271" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>16</v>
       </c>
@@ -36388,7 +36375,7 @@
         <v>75.599999999999994</v>
       </c>
     </row>
-    <row r="272" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>16</v>
       </c>
@@ -36438,7 +36425,7 @@
         <v>76.099999999999994</v>
       </c>
     </row>
-    <row r="273" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>16</v>
       </c>
@@ -36488,7 +36475,7 @@
         <v>76.3</v>
       </c>
     </row>
-    <row r="274" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>16</v>
       </c>
@@ -36538,7 +36525,7 @@
         <v>76.400000000000006</v>
       </c>
     </row>
-    <row r="275" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>16</v>
       </c>
@@ -36588,7 +36575,7 @@
         <v>75.400000000000006</v>
       </c>
     </row>
-    <row r="276" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>16</v>
       </c>
@@ -36638,7 +36625,7 @@
         <v>75.7</v>
       </c>
     </row>
-    <row r="277" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>16</v>
       </c>
@@ -36688,7 +36675,7 @@
         <v>75.2</v>
       </c>
     </row>
-    <row r="278" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>16</v>
       </c>
@@ -36738,7 +36725,7 @@
         <v>75.8</v>
       </c>
     </row>
-    <row r="279" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>16</v>
       </c>
@@ -36788,7 +36775,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="280" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>16</v>
       </c>
@@ -36838,7 +36825,7 @@
         <v>75.3</v>
       </c>
     </row>
-    <row r="281" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>16</v>
       </c>
@@ -36888,7 +36875,7 @@
         <v>75.2</v>
       </c>
     </row>
-    <row r="282" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>16</v>
       </c>
@@ -36938,7 +36925,7 @@
         <v>75.599999999999994</v>
       </c>
     </row>
-    <row r="283" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>16</v>
       </c>
@@ -36988,7 +36975,7 @@
         <v>75.3</v>
       </c>
     </row>
-    <row r="284" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>16</v>
       </c>
@@ -37038,7 +37025,7 @@
         <v>75.3</v>
       </c>
     </row>
-    <row r="285" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>16</v>
       </c>
@@ -37088,7 +37075,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="286" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>16</v>
       </c>
@@ -37138,7 +37125,7 @@
         <v>75.3</v>
       </c>
     </row>
-    <row r="287" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>16</v>
       </c>
@@ -37188,7 +37175,7 @@
         <v>75.400000000000006</v>
       </c>
     </row>
-    <row r="288" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>16</v>
       </c>
@@ -37238,7 +37225,7 @@
         <v>75.8</v>
       </c>
     </row>
-    <row r="289" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>16</v>
       </c>
@@ -37288,7 +37275,7 @@
         <v>74.7</v>
       </c>
     </row>
-    <row r="290" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>16</v>
       </c>
@@ -37338,7 +37325,7 @@
         <v>75.3</v>
       </c>
     </row>
-    <row r="291" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>16</v>
       </c>
@@ -37388,7 +37375,7 @@
         <v>74.400000000000006</v>
       </c>
     </row>
-    <row r="292" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>16</v>
       </c>
@@ -37438,7 +37425,7 @@
         <v>75.099999999999994</v>
       </c>
     </row>
-    <row r="293" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>16</v>
       </c>
@@ -37488,7 +37475,7 @@
         <v>75.2</v>
       </c>
     </row>
-    <row r="294" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>16</v>
       </c>
@@ -37538,7 +37525,7 @@
         <v>75.099999999999994</v>
       </c>
     </row>
-    <row r="295" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>16</v>
       </c>
@@ -37588,7 +37575,7 @@
         <v>74.3</v>
       </c>
     </row>
-    <row r="296" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>16</v>
       </c>
@@ -37638,7 +37625,7 @@
         <v>73.7</v>
       </c>
     </row>
-    <row r="297" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>16</v>
       </c>
@@ -37688,7 +37675,7 @@
         <v>74.599999999999994</v>
       </c>
     </row>
-    <row r="298" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>16</v>
       </c>
@@ -37738,7 +37725,7 @@
         <v>74.400000000000006</v>
       </c>
     </row>
-    <row r="299" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>16</v>
       </c>
@@ -37788,7 +37775,7 @@
         <v>74.3</v>
       </c>
     </row>
-    <row r="300" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>16</v>
       </c>
@@ -37838,7 +37825,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="301" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>16</v>
       </c>
@@ -37888,7 +37875,7 @@
         <v>73.400000000000006</v>
       </c>
     </row>
-    <row r="302" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>16</v>
       </c>
@@ -37938,7 +37925,7 @@
         <v>73.400000000000006</v>
       </c>
     </row>
-    <row r="303" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>16</v>
       </c>
@@ -37988,7 +37975,7 @@
         <v>73.599999999999994</v>
       </c>
     </row>
-    <row r="304" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>16</v>
       </c>
@@ -38038,7 +38025,7 @@
         <v>74.2</v>
       </c>
     </row>
-    <row r="305" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>16</v>
       </c>
@@ -38088,7 +38075,7 @@
         <v>74.599999999999994</v>
       </c>
     </row>
-    <row r="306" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>16</v>
       </c>
@@ -38138,7 +38125,7 @@
         <v>74.3</v>
       </c>
     </row>
-    <row r="307" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>16</v>
       </c>
@@ -38188,7 +38175,7 @@
         <v>74.3</v>
       </c>
     </row>
-    <row r="308" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>16</v>
       </c>
@@ -38238,7 +38225,7 @@
         <v>74.5</v>
       </c>
     </row>
-    <row r="309" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>16</v>
       </c>
@@ -38288,7 +38275,7 @@
         <v>74.7</v>
       </c>
     </row>
-    <row r="310" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>16</v>
       </c>
@@ -38338,7 +38325,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="311" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>16</v>
       </c>
@@ -38388,7 +38375,7 @@
         <v>74.2</v>
       </c>
     </row>
-    <row r="312" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>16</v>
       </c>
@@ -38438,7 +38425,7 @@
         <v>74.099999999999994</v>
       </c>
     </row>
-    <row r="313" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>16</v>
       </c>
@@ -38488,7 +38475,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="314" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>16</v>
       </c>
@@ -38538,7 +38525,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="315" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>16</v>
       </c>
@@ -38588,7 +38575,7 @@
         <v>72.2</v>
       </c>
     </row>
-    <row r="316" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>16</v>
       </c>
@@ -38638,7 +38625,7 @@
         <v>69.8</v>
       </c>
     </row>
-    <row r="317" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>16</v>
       </c>
@@ -38688,7 +38675,7 @@
         <v>70.900000000000006</v>
       </c>
     </row>
-    <row r="318" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>16</v>
       </c>
@@ -38738,7 +38725,7 @@
         <v>72.3</v>
       </c>
     </row>
-    <row r="319" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>16</v>
       </c>
@@ -38788,7 +38775,7 @@
         <v>72.3</v>
       </c>
     </row>
-    <row r="320" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>16</v>
       </c>
@@ -38838,7 +38825,7 @@
         <v>72.3</v>
       </c>
     </row>
-    <row r="321" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>16</v>
       </c>
@@ -38888,7 +38875,7 @@
         <v>72.7</v>
       </c>
     </row>
-    <row r="322" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>16</v>
       </c>
@@ -38938,7 +38925,7 @@
         <v>72.900000000000006</v>
       </c>
     </row>
-    <row r="323" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>16</v>
       </c>
@@ -38988,7 +38975,7 @@
         <v>72.8</v>
       </c>
     </row>
-    <row r="324" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>16</v>
       </c>
@@ -39038,7 +39025,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="325" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>16</v>
       </c>
@@ -39088,7 +39075,7 @@
         <v>72.5</v>
       </c>
     </row>
-    <row r="326" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>16</v>
       </c>
@@ -39138,7 +39125,7 @@
         <v>70.3</v>
       </c>
     </row>
-    <row r="327" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>16</v>
       </c>
@@ -39188,7 +39175,7 @@
         <v>68.900000000000006</v>
       </c>
     </row>
-    <row r="328" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>16</v>
       </c>
@@ -39238,7 +39225,7 @@
         <v>67.2</v>
       </c>
     </row>
-    <row r="329" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>16</v>
       </c>
@@ -39288,7 +39275,7 @@
         <v>65.8</v>
       </c>
     </row>
-    <row r="330" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>16</v>
       </c>
@@ -39338,7 +39325,7 @@
         <v>65.099999999999994</v>
       </c>
     </row>
-    <row r="331" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>16</v>
       </c>
@@ -39388,7 +39375,7 @@
         <v>64.900000000000006</v>
       </c>
     </row>
-    <row r="332" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>16</v>
       </c>
@@ -39438,7 +39425,7 @@
         <v>66.5</v>
       </c>
     </row>
-    <row r="333" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>16</v>
       </c>
@@ -39488,7 +39475,7 @@
         <v>68.599999999999994</v>
       </c>
     </row>
-    <row r="334" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>16</v>
       </c>
@@ -39538,7 +39525,7 @@
         <v>67.2</v>
       </c>
     </row>
-    <row r="335" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>16</v>
       </c>
@@ -39588,7 +39575,7 @@
         <v>65.3</v>
       </c>
     </row>
-    <row r="336" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>16</v>
       </c>
@@ -39638,7 +39625,7 @@
         <v>66.400000000000006</v>
       </c>
     </row>
-    <row r="337" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>16</v>
       </c>
@@ -39688,7 +39675,7 @@
         <v>67.900000000000006</v>
       </c>
     </row>
-    <row r="338" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>16</v>
       </c>
@@ -39738,7 +39725,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="339" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>16</v>
       </c>
@@ -39788,7 +39775,7 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="340" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>16</v>
       </c>
@@ -39838,7 +39825,7 @@
         <v>70.7</v>
       </c>
     </row>
-    <row r="341" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>16</v>
       </c>
@@ -39888,7 +39875,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="342" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>16</v>
       </c>
@@ -39938,7 +39925,7 @@
         <v>71.8</v>
       </c>
     </row>
-    <row r="343" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>16</v>
       </c>
@@ -39988,7 +39975,7 @@
         <v>71.2</v>
       </c>
     </row>
-    <row r="344" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>16</v>
       </c>
@@ -40038,7 +40025,7 @@
         <v>70.900000000000006</v>
       </c>
     </row>
-    <row r="345" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>16</v>
       </c>
@@ -40088,7 +40075,7 @@
         <v>71.3</v>
       </c>
     </row>
-    <row r="346" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>16</v>
       </c>
@@ -40138,7 +40125,7 @@
         <v>71.400000000000006</v>
       </c>
     </row>
-    <row r="347" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>16</v>
       </c>
@@ -40188,7 +40175,7 @@
         <v>71.5</v>
       </c>
     </row>
-    <row r="348" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>16</v>
       </c>
@@ -40238,7 +40225,7 @@
         <v>71.599999999999994</v>
       </c>
     </row>
-    <row r="349" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>16</v>
       </c>
@@ -40288,7 +40275,7 @@
         <v>71.2</v>
       </c>
     </row>
-    <row r="350" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>16</v>
       </c>
@@ -40338,7 +40325,7 @@
         <v>70.8</v>
       </c>
     </row>
-    <row r="351" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>16</v>
       </c>
@@ -40388,7 +40375,7 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="352" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>16</v>
       </c>
@@ -40438,7 +40425,7 @@
         <v>67.099999999999994</v>
       </c>
     </row>
-    <row r="353" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>16</v>
       </c>
@@ -40488,7 +40475,7 @@
         <v>66.599999999999994</v>
       </c>
     </row>
-    <row r="354" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>16</v>
       </c>
@@ -40538,7 +40525,7 @@
         <v>67.099999999999994</v>
       </c>
     </row>
-    <row r="355" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>16</v>
       </c>
@@ -40588,7 +40575,7 @@
         <v>67.900000000000006</v>
       </c>
     </row>
-    <row r="356" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>16</v>
       </c>
@@ -40638,7 +40625,7 @@
         <v>68.8</v>
       </c>
     </row>
-    <row r="357" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>16</v>
       </c>
@@ -40688,7 +40675,7 @@
         <v>70.099999999999994</v>
       </c>
     </row>
-    <row r="358" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>16</v>
       </c>
@@ -40738,7 +40725,7 @@
         <v>70.2</v>
       </c>
     </row>
-    <row r="359" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>16</v>
       </c>
@@ -40788,7 +40775,7 @@
         <v>69.400000000000006</v>
       </c>
     </row>
-    <row r="360" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>16</v>
       </c>
@@ -40838,7 +40825,7 @@
         <v>70.099999999999994</v>
       </c>
     </row>
-    <row r="361" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>16</v>
       </c>
@@ -40888,7 +40875,7 @@
         <v>70.7</v>
       </c>
     </row>
-    <row r="362" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>16</v>
       </c>
@@ -40938,7 +40925,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="363" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>16</v>
       </c>
@@ -40988,7 +40975,7 @@
         <v>70.7</v>
       </c>
     </row>
-    <row r="364" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>16</v>
       </c>
@@ -41038,7 +41025,7 @@
         <v>70.7</v>
       </c>
     </row>
-    <row r="365" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>16</v>
       </c>
@@ -41088,7 +41075,7 @@
         <v>70.8</v>
       </c>
     </row>
-    <row r="366" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>16</v>
       </c>
@@ -41138,7 +41125,7 @@
         <v>69.900000000000006</v>
       </c>
     </row>
-    <row r="367" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>16</v>
       </c>
@@ -41188,7 +41175,7 @@
         <v>70.2</v>
       </c>
     </row>
-    <row r="368" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>16</v>
       </c>
@@ -41238,7 +41225,7 @@
         <v>70.900000000000006</v>
       </c>
     </row>
-    <row r="369" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>16</v>
       </c>
@@ -41288,7 +41275,7 @@
         <v>70.8</v>
       </c>
     </row>
-    <row r="370" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>16</v>
       </c>
@@ -41338,7 +41325,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="371" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>16</v>
       </c>
@@ -41388,7 +41375,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="372" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>16</v>
       </c>
@@ -41438,7 +41425,7 @@
         <v>70.5</v>
       </c>
     </row>
-    <row r="373" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>16</v>
       </c>
@@ -41488,7 +41475,7 @@
         <v>70.7</v>
       </c>
     </row>
-    <row r="374" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>16</v>
       </c>
@@ -41538,7 +41525,7 @@
         <v>70.400000000000006</v>
       </c>
     </row>
-    <row r="375" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>16</v>
       </c>
@@ -41588,7 +41575,7 @@
         <v>70.3</v>
       </c>
     </row>
-    <row r="376" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>16</v>
       </c>
@@ -41638,7 +41625,7 @@
         <v>70.2</v>
       </c>
     </row>
-    <row r="377" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>16</v>
       </c>
@@ -41688,7 +41675,7 @@
         <v>70.400000000000006</v>
       </c>
     </row>
-    <row r="378" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>16</v>
       </c>
@@ -41738,7 +41725,7 @@
         <v>70.400000000000006</v>
       </c>
     </row>
-    <row r="379" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>16</v>
       </c>
@@ -41788,7 +41775,7 @@
         <v>70.400000000000006</v>
       </c>
     </row>
-    <row r="380" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>16</v>
       </c>
@@ -41838,7 +41825,7 @@
         <v>69.2</v>
       </c>
     </row>
-    <row r="381" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>16</v>
       </c>
@@ -41888,7 +41875,7 @@
         <v>69.099999999999994</v>
       </c>
     </row>
-    <row r="382" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>16</v>
       </c>
@@ -41938,7 +41925,7 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="383" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>16</v>
       </c>
@@ -41988,7 +41975,7 @@
         <v>68.2</v>
       </c>
     </row>
-    <row r="384" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>16</v>
       </c>
@@ -42038,7 +42025,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="385" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>16</v>
       </c>
@@ -42088,7 +42075,7 @@
         <v>67.7</v>
       </c>
     </row>
-    <row r="386" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>16</v>
       </c>
@@ -42138,7 +42125,7 @@
         <v>67.400000000000006</v>
       </c>
     </row>
-    <row r="387" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>16</v>
       </c>
@@ -42188,7 +42175,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="388" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>16</v>
       </c>
@@ -42238,7 +42225,7 @@
         <v>67.599999999999994</v>
       </c>
     </row>
-    <row r="389" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>16</v>
       </c>
@@ -42288,7 +42275,7 @@
         <v>67.8</v>
       </c>
     </row>
-    <row r="390" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>16</v>
       </c>
@@ -42338,7 +42325,7 @@
         <v>67.599999999999994</v>
       </c>
     </row>
-    <row r="391" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>16</v>
       </c>
@@ -42388,7 +42375,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="392" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>16</v>
       </c>
@@ -42438,7 +42425,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="393" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>16</v>
       </c>
@@ -42488,7 +42475,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="394" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>16</v>
       </c>
@@ -42538,7 +42525,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="395" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>16</v>
       </c>
@@ -42588,7 +42575,7 @@
         <v>67.099999999999994</v>
       </c>
     </row>
-    <row r="396" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>16</v>
       </c>
@@ -42638,7 +42625,7 @@
         <v>66.099999999999994</v>
       </c>
     </row>
-    <row r="397" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>16</v>
       </c>
@@ -42688,7 +42675,7 @@
         <v>66.400000000000006</v>
       </c>
     </row>
-    <row r="398" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>16</v>
       </c>
@@ -42738,7 +42725,7 @@
         <v>66.099999999999994</v>
       </c>
     </row>
-    <row r="399" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>16</v>
       </c>
@@ -42788,7 +42775,7 @@
         <v>66.099999999999994</v>
       </c>
     </row>
-    <row r="400" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>16</v>
       </c>
@@ -42838,7 +42825,7 @@
         <v>65.3</v>
       </c>
     </row>
-    <row r="401" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>16</v>
       </c>
@@ -42888,7 +42875,7 @@
         <v>64.5</v>
       </c>
     </row>
-    <row r="402" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>16</v>
       </c>
@@ -42938,7 +42925,7 @@
         <v>64.400000000000006</v>
       </c>
     </row>
-    <row r="403" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>16</v>
       </c>
@@ -42988,7 +42975,7 @@
         <v>64.2</v>
       </c>
     </row>
-    <row r="404" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>16</v>
       </c>
@@ -43038,7 +43025,7 @@
         <v>64.5</v>
       </c>
     </row>
-    <row r="405" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>16</v>
       </c>
@@ -43088,7 +43075,7 @@
         <v>64.599999999999994</v>
       </c>
     </row>
-    <row r="406" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>16</v>
       </c>
@@ -43138,7 +43125,7 @@
         <v>64.7</v>
       </c>
     </row>
-    <row r="407" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>16</v>
       </c>
@@ -43188,7 +43175,7 @@
         <v>64.599999999999994</v>
       </c>
     </row>
-    <row r="408" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>16</v>
       </c>
@@ -43238,7 +43225,7 @@
         <v>65.099999999999994</v>
       </c>
     </row>
-    <row r="409" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>16</v>
       </c>
@@ -43288,7 +43275,7 @@
         <v>64.8</v>
       </c>
     </row>
-    <row r="410" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>16</v>
       </c>
@@ -43338,7 +43325,7 @@
         <v>64.900000000000006</v>
       </c>
     </row>
-    <row r="411" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>16</v>
       </c>
@@ -43388,7 +43375,7 @@
         <v>64.900000000000006</v>
       </c>
     </row>
-    <row r="412" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>16</v>
       </c>
@@ -43438,7 +43425,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="413" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>16</v>
       </c>
@@ -43488,7 +43475,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="414" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>16</v>
       </c>
@@ -43538,7 +43525,7 @@
         <v>64.7</v>
       </c>
     </row>
-    <row r="415" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>16</v>
       </c>
@@ -43588,7 +43575,7 @@
         <v>64.5</v>
       </c>
     </row>
-    <row r="416" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>16</v>
       </c>
@@ -43638,7 +43625,7 @@
         <v>63.9</v>
       </c>
     </row>
-    <row r="417" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>16</v>
       </c>
@@ -43688,7 +43675,7 @@
         <v>64.099999999999994</v>
       </c>
     </row>
-    <row r="418" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>16</v>
       </c>
@@ -43738,7 +43725,7 @@
         <v>63.9</v>
       </c>
     </row>
-    <row r="419" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>16</v>
       </c>
@@ -43788,7 +43775,7 @@
         <v>63.5</v>
       </c>
     </row>
-    <row r="420" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>16</v>
       </c>
@@ -43838,7 +43825,7 @@
         <v>63.3</v>
       </c>
     </row>
-    <row r="421" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>16</v>
       </c>
@@ -43888,7 +43875,7 @@
         <v>63.3</v>
       </c>
     </row>
-    <row r="422" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>16</v>
       </c>
@@ -43938,7 +43925,7 @@
         <v>63.6</v>
       </c>
     </row>
-    <row r="423" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>16</v>
       </c>
@@ -43988,7 +43975,7 @@
         <v>63.5</v>
       </c>
     </row>
-    <row r="424" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>16</v>
       </c>
@@ -44038,7 +44025,7 @@
         <v>63.6</v>
       </c>
     </row>
-    <row r="425" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>16</v>
       </c>
@@ -44088,7 +44075,7 @@
         <v>63.1</v>
       </c>
     </row>
-    <row r="426" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>16</v>
       </c>
@@ -44138,7 +44125,7 @@
         <v>63.4</v>
       </c>
     </row>
-    <row r="427" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>16</v>
       </c>
@@ -44188,7 +44175,7 @@
         <v>62.7</v>
       </c>
     </row>
-    <row r="428" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>16</v>
       </c>
@@ -44238,7 +44225,7 @@
         <v>62.6</v>
       </c>
     </row>
-    <row r="429" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D429">
         <f>MIN(D2:D428)</f>
         <v>32.1</v>
@@ -44279,7 +44266,7 @@
         <v>42.031111111111116</v>
       </c>
     </row>
-    <row r="430" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D430">
         <f>MAX(D2:D429)</f>
         <v>69.099999999999994</v>
@@ -44317,7 +44304,7 @@
         <v>63.9</v>
       </c>
     </row>
-    <row r="431" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D431" s="6" t="s">
         <v>3</v>
       </c>
@@ -44346,17 +44333,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="433" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="434" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="435" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="436" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="531" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="531" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B531" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>